<commit_message>
feat: modify loginId type
</commit_message>
<xml_diff>
--- a/resources/excel/연구논문작품시스템_교수_일괄등록_양식.xlsx
+++ b/resources/excel/연구논문작품시스템_교수_일괄등록_양식.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hynseok/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dev_young_uk/real-ice-gs-thesis-backend/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69693392-E87E-5442-850B-8C68D5C8D1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B70ED8-D7AC-AF4C-AD0E-C58D0586A52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{043626C0-2E36-4A3C-83D7-8E6001ABEB02}"/>
+    <workbookView xWindow="6980" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{043626C0-2E36-4A3C-83D7-8E6001ABEB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>비밀번호</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>연락처</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>01099999999</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>내선번호</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -93,6 +85,22 @@
   </si>
   <si>
     <t>※ 수정 시에는 이미 존재하는 계정에 대해서만 가능하며 입력한 칸에 대해서만 수정이 이루어집니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인아이디</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginId1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginId2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010-9999-9999</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -210,7 +218,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -224,14 +232,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -550,7 +559,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D5" sqref="D4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -565,7 +574,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickTop="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -580,67 +589,67 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1">
-      <c r="A2" s="9">
-        <v>1111</v>
+      <c r="A2" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>1234</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="9">
-        <v>1112</v>
+      <c r="A3" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="B3">
         <v>1234</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:13">
       <c r="G4" s="1"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -650,8 +659,8 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="H6" s="10" t="s">
-        <v>13</v>
+      <c r="H6" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -660,15 +669,11 @@
     <row r="7" spans="1:13">
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{DC228F9C-3852-F14C-94DC-B2BF364D580F}"/>
-    <hyperlink ref="D3" r:id="rId2" display="prof1@example.com" xr:uid="{A785F84D-7308-9149-98E6-418FE326620F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: modify loginId type (#105)
* feat: modify loginId type

* feat: modify loginId type 2

* chore: 엑셀양식 참고사항 수정

---------

Co-authored-by: hynseok <wefwef12e@naver.com>
</commit_message>
<xml_diff>
--- a/resources/excel/연구논문작품시스템_교수_일괄등록_양식.xlsx
+++ b/resources/excel/연구논문작품시스템_교수_일괄등록_양식.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hynseok/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hynseok/Projects/scg/temp/real-ice-gs-thesis-backend/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69693392-E87E-5442-850B-8C68D5C8D1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B52DBD-6125-B344-A891-56E84DBBFF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{043626C0-2E36-4A3C-83D7-8E6001ABEB02}"/>
+    <workbookView xWindow="6980" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{043626C0-2E36-4A3C-83D7-8E6001ABEB02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>비밀번호</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -51,14 +51,6 @@
   </si>
   <si>
     <t>연락처</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>01099999999</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>내선번호</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -93,6 +85,22 @@
   </si>
   <si>
     <t>※ 수정 시에는 이미 존재하는 계정에 대해서만 가능하며 입력한 칸에 대해서만 수정이 이루어집니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인아이디</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginId1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginId2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010-9999-9999</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -100,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +163,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
@@ -224,14 +239,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -549,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6009F09-5088-44C3-9E9B-7575341D7EF8}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -565,7 +582,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="19" thickTop="1" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -580,67 +597,67 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickTop="1">
-      <c r="A2" s="9">
-        <v>1111</v>
+      <c r="A2" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>1234</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="9">
-        <v>1112</v>
+      <c r="A3" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="B3">
         <v>1234</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:13">
       <c r="G4" s="1"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -649,9 +666,9 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" ht="20">
       <c r="H6" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -660,15 +677,11 @@
     <row r="7" spans="1:13">
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{DC228F9C-3852-F14C-94DC-B2BF364D580F}"/>
-    <hyperlink ref="D3" r:id="rId2" display="prof1@example.com" xr:uid="{A785F84D-7308-9149-98E6-418FE326620F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>